<commit_message>
Backup to GitHub - 2021.05.15
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
+++ b/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
@@ -471,37 +471,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.85</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C2">
         <v>0.84</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="I2">
-        <v>0.71</v>
+        <v>0.82</v>
       </c>
       <c r="J2">
-        <v>0.71</v>
+        <v>0.74</v>
       </c>
       <c r="K2">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="L2">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -509,37 +509,37 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.97</v>
+        <v>0.86</v>
       </c>
       <c r="C3">
-        <v>0.82</v>
+        <v>0.77</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>0.75</v>
+        <v>0.57</v>
       </c>
       <c r="I3">
-        <v>0.53</v>
+        <v>0.76</v>
       </c>
       <c r="J3">
-        <v>0.62</v>
+        <v>0.65</v>
       </c>
       <c r="K3">
-        <v>0.93</v>
+        <v>0.78</v>
       </c>
       <c r="L3">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -547,37 +547,37 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.87</v>
+        <v>0.82</v>
       </c>
       <c r="C4">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>0.75</v>
+        <v>0.67</v>
       </c>
       <c r="I4">
-        <v>0.71</v>
+        <v>0.82</v>
       </c>
       <c r="J4">
-        <v>0.73</v>
+        <v>0.74</v>
       </c>
       <c r="K4">
-        <v>0.91</v>
+        <v>0.84</v>
       </c>
       <c r="L4">
-        <v>0.8100000000000001</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -585,37 +585,37 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.9399999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="C5">
         <v>0.84</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="I5">
-        <v>0.65</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J5">
-        <v>0.6899999999999999</v>
+        <v>0.76</v>
       </c>
       <c r="K5">
-        <v>0.91</v>
+        <v>0.8</v>
       </c>
       <c r="L5">
-        <v>0.78</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -626,34 +626,34 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.85</v>
+        <v>0.79</v>
       </c>
       <c r="D6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.54</v>
+        <v>0.61</v>
       </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.76</v>
+      </c>
+      <c r="K6">
+        <v>0.76</v>
+      </c>
+      <c r="L6">
         <v>0.88</v>
-      </c>
-      <c r="J6">
-        <v>0.67</v>
-      </c>
-      <c r="K6">
-        <v>0.71</v>
-      </c>
-      <c r="L6">
-        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup to GitHub - 2021.05.18
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
+++ b/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
@@ -471,37 +471,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.8100000000000001</v>
+        <v>0.87</v>
       </c>
       <c r="C2">
-        <v>0.84</v>
+        <v>0.77</v>
       </c>
       <c r="D2">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>0.67</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I2">
-        <v>0.82</v>
+        <v>0.55</v>
       </c>
       <c r="J2">
-        <v>0.74</v>
+        <v>0.61</v>
       </c>
       <c r="K2">
-        <v>0.84</v>
+        <v>0.88</v>
       </c>
       <c r="L2">
-        <v>0.83</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -509,37 +509,37 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.86</v>
+        <v>0.98</v>
       </c>
       <c r="C3">
         <v>0.77</v>
       </c>
       <c r="D3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
       <c r="H3">
-        <v>0.57</v>
+        <v>0.71</v>
       </c>
       <c r="I3">
-        <v>0.76</v>
+        <v>0.5</v>
       </c>
       <c r="J3">
-        <v>0.65</v>
+        <v>0.59</v>
       </c>
       <c r="K3">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
       <c r="L3">
-        <v>0.77</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -547,37 +547,37 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.82</v>
+        <v>0.88</v>
       </c>
       <c r="C4">
-        <v>0.84</v>
+        <v>0.78</v>
       </c>
       <c r="D4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H4">
-        <v>0.67</v>
+        <v>0.73</v>
       </c>
       <c r="I4">
-        <v>0.82</v>
+        <v>0.55</v>
       </c>
       <c r="J4">
-        <v>0.74</v>
+        <v>0.63</v>
       </c>
       <c r="K4">
-        <v>0.84</v>
+        <v>0.9</v>
       </c>
       <c r="L4">
-        <v>0.83</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -585,37 +585,37 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.86</v>
+        <v>0.95</v>
       </c>
       <c r="C5">
-        <v>0.84</v>
+        <v>0.78</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>36</v>
       </c>
       <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <v>9</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
       <c r="H5">
-        <v>0.64</v>
+        <v>0.73</v>
       </c>
       <c r="I5">
-        <v>0.9399999999999999</v>
+        <v>0.55</v>
       </c>
       <c r="J5">
-        <v>0.76</v>
+        <v>0.63</v>
       </c>
       <c r="K5">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="L5">
-        <v>0.87</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -623,37 +623,37 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="C6">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
         <v>34</v>
-      </c>
-      <c r="F6">
-        <v>11</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0.61</v>
+        <v>0.37</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0.76</v>
+        <v>0.54</v>
       </c>
       <c r="K6">
-        <v>0.76</v>
+        <v>0.15</v>
       </c>
       <c r="L6">
-        <v>0.88</v>
+        <v>0.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup to GitHub - 2021.05.22
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
+++ b/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
@@ -471,37 +471,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.83</v>
+        <v>0.87</v>
       </c>
       <c r="C2">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
       <c r="D2">
         <v>13</v>
       </c>
       <c r="E2">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>4</v>
       </c>
       <c r="H2">
-        <v>0.65</v>
+        <v>0.68</v>
       </c>
       <c r="I2">
         <v>0.76</v>
       </c>
       <c r="J2">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
       <c r="K2">
-        <v>0.84</v>
+        <v>0.87</v>
       </c>
       <c r="L2">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -509,37 +509,37 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="C3">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>0.77</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I3">
-        <v>0.59</v>
+        <v>0.65</v>
       </c>
       <c r="J3">
         <v>0.67</v>
       </c>
       <c r="K3">
-        <v>0.93</v>
+        <v>0.89</v>
       </c>
       <c r="L3">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -547,37 +547,37 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
       <c r="C4">
         <v>0.85</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>0.75</v>
+        <v>0.68</v>
       </c>
       <c r="I4">
-        <v>0.71</v>
+        <v>0.88</v>
       </c>
       <c r="J4">
-        <v>0.73</v>
+        <v>0.77</v>
       </c>
       <c r="K4">
-        <v>0.91</v>
+        <v>0.84</v>
       </c>
       <c r="L4">
-        <v>0.8100000000000001</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -585,37 +585,37 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="C5">
-        <v>0.76</v>
+        <v>0.84</v>
       </c>
       <c r="D5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F5">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>0.54</v>
+        <v>0.73</v>
       </c>
       <c r="I5">
-        <v>0.76</v>
+        <v>0.65</v>
       </c>
       <c r="J5">
-        <v>0.63</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="K5">
-        <v>0.76</v>
+        <v>0.91</v>
       </c>
       <c r="L5">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -623,37 +623,37 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="C6">
-        <v>0.77</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D6">
         <v>15</v>
       </c>
       <c r="E6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6">
-        <v>0.54</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="I6">
         <v>0.88</v>
       </c>
       <c r="J6">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="K6">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
       <c r="L6">
-        <v>0.8</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup to GitHub - 2021.06.11
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
+++ b/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
@@ -471,13 +471,13 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.87</v>
+        <v>0.85</v>
       </c>
       <c r="C2">
-        <v>0.84</v>
+        <v>0.82</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>39</v>
@@ -486,22 +486,22 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="I2">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="J2">
-        <v>0.72</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="K2">
         <v>0.87</v>
       </c>
       <c r="L2">
-        <v>0.82</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -509,37 +509,37 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
       <c r="C3">
-        <v>0.84</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H3">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
       <c r="I3">
-        <v>0.71</v>
+        <v>0.47</v>
       </c>
       <c r="J3">
-        <v>0.71</v>
+        <v>0.57</v>
       </c>
       <c r="K3">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
       <c r="L3">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -547,37 +547,37 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="C4">
-        <v>0.85</v>
+        <v>0.82</v>
       </c>
       <c r="D4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="I4">
-        <v>0.88</v>
+        <v>0.71</v>
       </c>
       <c r="J4">
-        <v>0.77</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="K4">
-        <v>0.84</v>
+        <v>0.87</v>
       </c>
       <c r="L4">
-        <v>0.86</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -585,37 +585,37 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="C5">
         <v>0.84</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="I5">
-        <v>0.65</v>
+        <v>0.71</v>
       </c>
       <c r="J5">
-        <v>0.6899999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="K5">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="L5">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -623,37 +623,37 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
       <c r="C6">
-        <v>0.79</v>
+        <v>0.84</v>
       </c>
       <c r="D6">
         <v>17</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F6">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0.29</v>
+        <v>0.33</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="K6">
-        <v>0.09</v>
+        <v>0.24</v>
       </c>
       <c r="L6">
-        <v>0.54</v>
+        <v>0.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup to GitHub - 2021.07.04
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
+++ b/01_Classification/03_Output/Back_Pain_MLM_Evaluation_Clf.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Model_Name</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>DNN</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
   <si>
     <t>precision</t>
@@ -514,37 +517,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.88</v>
+        <v>0.86</v>
       </c>
       <c r="C2">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
       <c r="D2">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
         <v>4</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
       </c>
       <c r="H2">
         <v>0.89</v>
       </c>
       <c r="I2">
-        <v>0.76</v>
+        <v>0.91</v>
       </c>
       <c r="J2">
-        <v>0.82</v>
+        <v>0.9</v>
       </c>
       <c r="K2">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="L2">
-        <v>0.78</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -552,37 +555,37 @@
         <v>13</v>
       </c>
       <c r="B3">
+        <v>0.95</v>
+      </c>
+      <c r="C3">
+        <v>0.82</v>
+      </c>
+      <c r="D3">
+        <v>43</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0.83</v>
+      </c>
+      <c r="I3">
         <v>0.96</v>
       </c>
-      <c r="C3">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="D3">
-        <v>34</v>
-      </c>
-      <c r="E3">
-        <v>16</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>8</v>
-      </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.89</v>
       </c>
-      <c r="I3">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="J3">
-        <v>0.85</v>
-      </c>
       <c r="K3">
-        <v>0.8</v>
+        <v>0.47</v>
       </c>
       <c r="L3">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -590,37 +593,37 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="C4">
         <v>0.82</v>
       </c>
       <c r="D4">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E4">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
       <c r="H4">
-        <v>0.92</v>
+        <v>0.84</v>
       </c>
       <c r="I4">
-        <v>0.8100000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="J4">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="K4">
-        <v>0.85</v>
+        <v>0.53</v>
       </c>
       <c r="L4">
-        <v>0.83</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -628,37 +631,37 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.98</v>
+        <v>0.85</v>
       </c>
       <c r="C5">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="D5">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>13</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H5">
+        <v>0.91</v>
+      </c>
+      <c r="I5">
+        <v>0.89</v>
+      </c>
+      <c r="J5">
+        <v>0.9</v>
+      </c>
+      <c r="K5">
+        <v>0.76</v>
+      </c>
+      <c r="L5">
         <v>0.83</v>
-      </c>
-      <c r="I5">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="J5">
-        <v>0.82</v>
-      </c>
-      <c r="K5">
-        <v>0.65</v>
-      </c>
-      <c r="L5">
-        <v>0.73</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -669,34 +672,34 @@
         <v>0.95</v>
       </c>
       <c r="C6">
-        <v>0.8100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E6">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>0.9399999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="I6">
+        <v>0.93</v>
+      </c>
+      <c r="J6">
+        <v>0.89</v>
+      </c>
+      <c r="K6">
+        <v>0.59</v>
+      </c>
+      <c r="L6">
         <v>0.76</v>
-      </c>
-      <c r="J6">
-        <v>0.84</v>
-      </c>
-      <c r="K6">
-        <v>0.9</v>
-      </c>
-      <c r="L6">
-        <v>0.83</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -704,37 +707,37 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0.95</v>
+        <v>0.86</v>
       </c>
       <c r="C7">
-        <v>0.77</v>
+        <v>0.84</v>
       </c>
       <c r="D7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>31</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
       </c>
       <c r="I7">
-        <v>0.26</v>
-      </c>
-      <c r="J7">
-        <v>0.41</v>
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0.63</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -752,36 +755,36 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="D2">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="E2">
-        <v>0.7</v>
+        <v>0.73</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -793,46 +796,46 @@
         <v>0.89</v>
       </c>
       <c r="D3">
-        <v>0.76</v>
+        <v>0.91</v>
       </c>
       <c r="E3">
-        <v>0.82</v>
+        <v>0.9</v>
       </c>
       <c r="F3">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
       <c r="D4">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
       <c r="E4">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
       <c r="F4">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>0.75</v>
+        <v>0.82</v>
       </c>
       <c r="D5">
-        <v>0.78</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E5">
-        <v>0.76</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F5">
         <v>62</v>
@@ -841,16 +844,16 @@
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="D6">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
       <c r="E6">
-        <v>0.78</v>
+        <v>0.85</v>
       </c>
       <c r="F6">
         <v>62</v>
@@ -858,22 +861,22 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.67</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
-        <v>0.8</v>
+        <v>0.47</v>
       </c>
       <c r="E7">
-        <v>0.73</v>
+        <v>0.59</v>
       </c>
       <c r="F7">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -882,49 +885,49 @@
         <v>1</v>
       </c>
       <c r="C8">
+        <v>0.83</v>
+      </c>
+      <c r="D8">
+        <v>0.96</v>
+      </c>
+      <c r="E8">
         <v>0.89</v>
       </c>
-      <c r="D8">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="E8">
-        <v>0.85</v>
-      </c>
       <c r="F8">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="D9">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="E9">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="F9">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>0.78</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D10">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="E10">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="F10">
         <v>62</v>
@@ -933,13 +936,13 @@
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>0.82</v>
       </c>
       <c r="D11">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="E11">
         <v>0.8100000000000001</v>
@@ -950,22 +953,22 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0.67</v>
+        <v>0.8</v>
       </c>
       <c r="D12">
-        <v>0.8</v>
+        <v>0.47</v>
       </c>
       <c r="E12">
-        <v>0.73</v>
+        <v>0.59</v>
       </c>
       <c r="F12">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -974,49 +977,49 @@
         <v>1</v>
       </c>
       <c r="C13">
+        <v>0.83</v>
+      </c>
+      <c r="D13">
+        <v>0.96</v>
+      </c>
+      <c r="E13">
         <v>0.89</v>
       </c>
-      <c r="D13">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="E13">
-        <v>0.85</v>
-      </c>
       <c r="F13">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="D14">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="E14">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="F14">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15">
-        <v>0.78</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D15">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="E15">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="F15">
         <v>62</v>
@@ -1025,13 +1028,13 @@
     <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>0.82</v>
       </c>
       <c r="D16">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="E16">
         <v>0.8100000000000001</v>
@@ -1042,22 +1045,22 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0.62</v>
+        <v>0.72</v>
       </c>
       <c r="D17">
-        <v>0.65</v>
+        <v>0.76</v>
       </c>
       <c r="E17">
-        <v>0.63</v>
+        <v>0.74</v>
       </c>
       <c r="F17">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1066,49 +1069,49 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0.83</v>
+        <v>0.91</v>
       </c>
       <c r="D18">
-        <v>0.8100000000000001</v>
+        <v>0.89</v>
       </c>
       <c r="E18">
-        <v>0.82</v>
+        <v>0.9</v>
       </c>
       <c r="F18">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="D19">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="E19">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="F19">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C20">
-        <v>0.72</v>
+        <v>0.82</v>
       </c>
       <c r="D20">
-        <v>0.73</v>
+        <v>0.83</v>
       </c>
       <c r="E20">
-        <v>0.73</v>
+        <v>0.82</v>
       </c>
       <c r="F20">
         <v>62</v>
@@ -1117,16 +1120,16 @@
     <row r="21" spans="1:6">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21">
-        <v>0.76</v>
+        <v>0.86</v>
       </c>
       <c r="D21">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="E21">
-        <v>0.76</v>
+        <v>0.86</v>
       </c>
       <c r="F21">
         <v>62</v>
@@ -1134,22 +1137,22 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.64</v>
+        <v>0.77</v>
       </c>
       <c r="D22">
-        <v>0.9</v>
+        <v>0.59</v>
       </c>
       <c r="E22">
-        <v>0.75</v>
+        <v>0.67</v>
       </c>
       <c r="F22">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1158,49 +1161,49 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0.9399999999999999</v>
+        <v>0.86</v>
       </c>
       <c r="D23">
-        <v>0.76</v>
+        <v>0.93</v>
       </c>
       <c r="E23">
-        <v>0.84</v>
+        <v>0.89</v>
       </c>
       <c r="F23">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C24">
-        <v>0.8100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="D24">
-        <v>0.8100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="E24">
-        <v>0.8100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="F24">
-        <v>0.8100000000000001</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C25">
-        <v>0.79</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D25">
-        <v>0.83</v>
+        <v>0.76</v>
       </c>
       <c r="E25">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="F25">
         <v>62</v>
@@ -1209,16 +1212,16 @@
     <row r="26" spans="1:6">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C26">
+        <v>0.83</v>
+      </c>
+      <c r="D26">
         <v>0.84</v>
       </c>
-      <c r="D26">
-        <v>0.8100000000000001</v>
-      </c>
       <c r="E26">
-        <v>0.8100000000000001</v>
+        <v>0.83</v>
       </c>
       <c r="F26">
         <v>62</v>
@@ -1226,22 +1229,22 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>0.39</v>
+        <v>0.27</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>0.5600000000000001</v>
+        <v>0.43</v>
       </c>
       <c r="F27">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1250,49 +1253,49 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>0.26</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0.42</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29">
-        <v>0.5</v>
+        <v>0.27</v>
       </c>
       <c r="D29">
-        <v>0.5</v>
+        <v>0.27</v>
       </c>
       <c r="E29">
-        <v>0.5</v>
+        <v>0.27</v>
       </c>
       <c r="F29">
-        <v>0.5</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30">
-        <v>0.7</v>
+        <v>0.14</v>
       </c>
       <c r="D30">
-        <v>0.63</v>
+        <v>0.5</v>
       </c>
       <c r="E30">
-        <v>0.49</v>
+        <v>0.22</v>
       </c>
       <c r="F30">
         <v>62</v>
@@ -1301,16 +1304,16 @@
     <row r="31" spans="1:6">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31">
-        <v>0.8</v>
+        <v>0.08</v>
       </c>
       <c r="D31">
-        <v>0.5</v>
+        <v>0.27</v>
       </c>
       <c r="E31">
-        <v>0.46</v>
+        <v>0.12</v>
       </c>
       <c r="F31">
         <v>62</v>

</xml_diff>